<commit_message>
finished code, output in thesis
</commit_message>
<xml_diff>
--- a/RandomForest_output_1.xlsx
+++ b/RandomForest_output_1.xlsx
@@ -485,7 +485,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>807.4598333333334</v>
+        <v>807.4598333333333</v>
       </c>
     </row>
     <row r="8">
@@ -501,7 +501,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>284.4251666666666</v>
+        <v>284.4251666666667</v>
       </c>
     </row>
     <row r="10">
@@ -509,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>500.4863333333334</v>
+        <v>500.4863333333333</v>
       </c>
     </row>
     <row r="11">
@@ -533,7 +533,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>448.08825</v>
+        <v>448.0882500000001</v>
       </c>
     </row>
     <row r="14">
@@ -541,7 +541,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>278.5315555555556</v>
+        <v>278.5315555555555</v>
       </c>
     </row>
     <row r="15">
@@ -597,7 +597,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>363.7166666666667</v>
+        <v>363.7166666666666</v>
       </c>
     </row>
     <row r="22">
@@ -621,7 +621,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>340.2853888888889</v>
+        <v>340.285388888889</v>
       </c>
     </row>
     <row r="25">
@@ -661,7 +661,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>292.5783888888887</v>
+        <v>292.5783888888888</v>
       </c>
     </row>
     <row r="30">
@@ -701,7 +701,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>396.536</v>
+        <v>396.5359999999999</v>
       </c>
     </row>
     <row r="35">
@@ -805,7 +805,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>302.9873333333333</v>
+        <v>302.9873333333334</v>
       </c>
     </row>
     <row r="48">
@@ -869,7 +869,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>321.75</v>
+        <v>321.7499999999999</v>
       </c>
     </row>
     <row r="56">
@@ -885,7 +885,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>799.1961111111111</v>
+        <v>799.1961111111112</v>
       </c>
     </row>
     <row r="58">
@@ -941,7 +941,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>332.3635</v>
+        <v>332.3634999999999</v>
       </c>
     </row>
     <row r="65">
@@ -1005,7 +1005,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>361.1740000000001</v>
+        <v>361.174</v>
       </c>
     </row>
     <row r="73">
@@ -1053,7 +1053,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>448.08825</v>
+        <v>448.0882500000001</v>
       </c>
     </row>
     <row r="79">
@@ -1061,7 +1061,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>751.8658333333333</v>
+        <v>751.8658333333334</v>
       </c>
     </row>
     <row r="80">
@@ -1093,7 +1093,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>393.7813333333335</v>
+        <v>393.7813333333334</v>
       </c>
     </row>
     <row r="84">
@@ -1149,7 +1149,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>1243.136166666667</v>
+        <v>1243.136166666666</v>
       </c>
     </row>
     <row r="91">
@@ -1245,7 +1245,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>372.8498888888889</v>
+        <v>372.8498888888888</v>
       </c>
     </row>
     <row r="103">
@@ -1333,7 +1333,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>230.3277777777779</v>
+        <v>230.327777777778</v>
       </c>
     </row>
     <row r="114">
@@ -1341,7 +1341,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>372.8498888888889</v>
+        <v>372.8498888888888</v>
       </c>
     </row>
     <row r="115">
@@ -1389,7 +1389,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>639.6166666666667</v>
+        <v>639.6166666666666</v>
       </c>
     </row>
     <row r="121">
@@ -1413,7 +1413,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>317.7350000000001</v>
+        <v>317.735</v>
       </c>
     </row>
     <row r="124">
@@ -1517,7 +1517,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>297.5833333333334</v>
+        <v>297.5833333333335</v>
       </c>
     </row>
     <row r="137">
@@ -1557,7 +1557,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>417.4206428571428</v>
+        <v>417.4206428571429</v>
       </c>
     </row>
     <row r="142">
@@ -1565,7 +1565,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>211.2</v>
+        <v>211.2000000000002</v>
       </c>
     </row>
     <row r="143">
@@ -1589,7 +1589,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>263.95</v>
+        <v>263.9500000000001</v>
       </c>
     </row>
     <row r="146">
@@ -1621,7 +1621,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>818.15</v>
+        <v>818.1499999999999</v>
       </c>
     </row>
     <row r="150">
@@ -1629,7 +1629,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>165.7166666666668</v>
+        <v>165.7166666666667</v>
       </c>
     </row>
     <row r="151">
@@ -1653,7 +1653,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>213.1833333333334</v>
+        <v>213.1833333333335</v>
       </c>
     </row>
     <row r="154">
@@ -1669,7 +1669,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>443.9733333333332</v>
+        <v>443.9733333333333</v>
       </c>
     </row>
     <row r="156">
@@ -1725,7 +1725,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>356.4346666666666</v>
+        <v>356.4346666666667</v>
       </c>
     </row>
     <row r="163">
@@ -1733,7 +1733,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>483.4712777777778</v>
+        <v>483.4712777777777</v>
       </c>
     </row>
     <row r="164">
@@ -1837,7 +1837,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>735.1555555555556</v>
+        <v>735.1555555555557</v>
       </c>
     </row>
     <row r="177">
@@ -1845,7 +1845,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>386.7258333333333</v>
+        <v>386.7258333333334</v>
       </c>
     </row>
     <row r="178">
@@ -1981,7 +1981,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>352.375</v>
+        <v>352.3750000000001</v>
       </c>
     </row>
     <row r="195">
@@ -1989,7 +1989,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>754.7139999999999</v>
+        <v>754.7140000000001</v>
       </c>
     </row>
     <row r="196">
@@ -2045,7 +2045,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>375.7242539682539</v>
+        <v>375.7242539682541</v>
       </c>
     </row>
     <row r="203">
@@ -2053,7 +2053,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>278.6858333333332</v>
+        <v>278.6858333333333</v>
       </c>
     </row>
     <row r="204">
@@ -2061,7 +2061,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>311.7260555555556</v>
+        <v>311.7260555555555</v>
       </c>
     </row>
     <row r="205">
@@ -2077,7 +2077,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>422.3966666666667</v>
+        <v>422.3966666666666</v>
       </c>
     </row>
     <row r="207">
@@ -2221,7 +2221,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="n">
-        <v>428.5841111111112</v>
+        <v>428.5841111111111</v>
       </c>
     </row>
     <row r="225">
@@ -2269,7 +2269,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="n">
-        <v>654.8405555555555</v>
+        <v>654.8405555555556</v>
       </c>
     </row>
     <row r="231">
@@ -2277,7 +2277,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>448.7450000000001</v>
+        <v>448.745</v>
       </c>
     </row>
     <row r="232">
@@ -2293,7 +2293,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>302.1614444444447</v>
+        <v>302.1614444444446</v>
       </c>
     </row>
     <row r="234">
@@ -2397,7 +2397,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="n">
-        <v>391.4603333333334</v>
+        <v>391.4603333333333</v>
       </c>
     </row>
     <row r="247">
@@ -2589,7 +2589,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="n">
-        <v>280.9666666666667</v>
+        <v>280.9666666666666</v>
       </c>
     </row>
     <row r="271">
@@ -2653,7 +2653,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="n">
-        <v>802.7666666666668</v>
+        <v>802.7666666666667</v>
       </c>
     </row>
     <row r="279">
@@ -2693,7 +2693,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="n">
-        <v>212.9896666666666</v>
+        <v>212.9896666666665</v>
       </c>
     </row>
     <row r="284">
@@ -2733,7 +2733,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="n">
-        <v>280.1008333333333</v>
+        <v>280.1008333333334</v>
       </c>
     </row>
     <row r="289">
@@ -2765,7 +2765,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="n">
-        <v>418.714</v>
+        <v>418.7140000000001</v>
       </c>
     </row>
     <row r="293">
@@ -2837,7 +2837,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="n">
-        <v>210.9333333333334</v>
+        <v>210.9333333333335</v>
       </c>
     </row>
     <row r="302">
@@ -2845,7 +2845,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="n">
-        <v>287.0601111111111</v>
+        <v>287.0601111111112</v>
       </c>
     </row>
     <row r="303">
@@ -2989,7 +2989,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="n">
-        <v>472.3176666666667</v>
+        <v>472.3176666666666</v>
       </c>
     </row>
     <row r="321">
@@ -2997,7 +2997,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="n">
-        <v>252.5277777777777</v>
+        <v>252.5277777777778</v>
       </c>
     </row>
     <row r="322">
@@ -3077,7 +3077,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="n">
-        <v>911.3164999999998</v>
+        <v>911.3164999999999</v>
       </c>
     </row>
     <row r="332">
@@ -3189,7 +3189,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="n">
-        <v>238.7333333333335</v>
+        <v>238.7333333333334</v>
       </c>
     </row>
     <row r="346">
@@ -3261,7 +3261,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="n">
-        <v>401.1906666666666</v>
+        <v>401.1906666666667</v>
       </c>
     </row>
     <row r="355">
@@ -3301,7 +3301,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="n">
-        <v>384.9458333333333</v>
+        <v>384.9458333333332</v>
       </c>
     </row>
     <row r="360">
@@ -3325,7 +3325,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="n">
-        <v>925.4279999999999</v>
+        <v>925.4280000000001</v>
       </c>
     </row>
     <row r="363">
@@ -3349,7 +3349,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="n">
-        <v>912.0911904761906</v>
+        <v>912.0911904761907</v>
       </c>
     </row>
     <row r="366">
@@ -3389,7 +3389,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="n">
-        <v>757.5124999999999</v>
+        <v>757.5125</v>
       </c>
     </row>
     <row r="371">
@@ -3461,7 +3461,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="n">
-        <v>397.4091111111112</v>
+        <v>397.4091111111111</v>
       </c>
     </row>
     <row r="380">
@@ -3469,7 +3469,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="n">
-        <v>326.4974999999999</v>
+        <v>326.4975</v>
       </c>
     </row>
     <row r="381">
@@ -3477,7 +3477,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="n">
-        <v>2694.713305555555</v>
+        <v>2694.713305555554</v>
       </c>
     </row>
     <row r="382">
@@ -3541,7 +3541,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="n">
-        <v>493.8283333333333</v>
+        <v>493.8283333333334</v>
       </c>
     </row>
     <row r="390">
@@ -3645,7 +3645,7 @@
         <v>400</v>
       </c>
       <c r="B402" t="n">
-        <v>610.3171666666666</v>
+        <v>610.3171666666667</v>
       </c>
     </row>
     <row r="403">
@@ -3669,7 +3669,7 @@
         <v>403</v>
       </c>
       <c r="B405" t="n">
-        <v>654.7166666666666</v>
+        <v>654.7166666666665</v>
       </c>
     </row>
     <row r="406">
@@ -3749,7 +3749,7 @@
         <v>413</v>
       </c>
       <c r="B415" t="n">
-        <v>529.3853333333334</v>
+        <v>529.3853333333333</v>
       </c>
     </row>
     <row r="416">
@@ -3765,7 +3765,7 @@
         <v>415</v>
       </c>
       <c r="B417" t="n">
-        <v>809.535</v>
+        <v>809.5349999999999</v>
       </c>
     </row>
     <row r="418">
@@ -3781,7 +3781,7 @@
         <v>417</v>
       </c>
       <c r="B419" t="n">
-        <v>839.9141666666667</v>
+        <v>839.9141666666668</v>
       </c>
     </row>
     <row r="420">
@@ -3821,7 +3821,7 @@
         <v>422</v>
       </c>
       <c r="B424" t="n">
-        <v>441.6993333333335</v>
+        <v>441.6993333333334</v>
       </c>
     </row>
     <row r="425">
@@ -3877,7 +3877,7 @@
         <v>429</v>
       </c>
       <c r="B431" t="n">
-        <v>962.7798333333333</v>
+        <v>962.7798333333334</v>
       </c>
     </row>
     <row r="432">
@@ -3893,7 +3893,7 @@
         <v>431</v>
       </c>
       <c r="B433" t="n">
-        <v>827.7549999999999</v>
+        <v>827.755</v>
       </c>
     </row>
     <row r="434">
@@ -3909,7 +3909,7 @@
         <v>433</v>
       </c>
       <c r="B435" t="n">
-        <v>596.6377555555556</v>
+        <v>596.6377555555555</v>
       </c>
     </row>
     <row r="436">
@@ -3941,7 +3941,7 @@
         <v>437</v>
       </c>
       <c r="B439" t="n">
-        <v>256.2191666666667</v>
+        <v>256.2191666666666</v>
       </c>
     </row>
     <row r="440">
@@ -3989,7 +3989,7 @@
         <v>443</v>
       </c>
       <c r="B445" t="n">
-        <v>391.0890000000001</v>
+        <v>391.089</v>
       </c>
     </row>
     <row r="446">
@@ -4037,7 +4037,7 @@
         <v>449</v>
       </c>
       <c r="B451" t="n">
-        <v>164.6208333333332</v>
+        <v>164.6208333333333</v>
       </c>
     </row>
     <row r="452">
@@ -4077,7 +4077,7 @@
         <v>454</v>
       </c>
       <c r="B456" t="n">
-        <v>793.4431111111113</v>
+        <v>793.4431111111114</v>
       </c>
     </row>
     <row r="457">
@@ -4093,7 +4093,7 @@
         <v>456</v>
       </c>
       <c r="B458" t="n">
-        <v>375.9598333333333</v>
+        <v>375.9598333333332</v>
       </c>
     </row>
     <row r="459">
@@ -4261,7 +4261,7 @@
         <v>477</v>
       </c>
       <c r="B479" t="n">
-        <v>912.0911904761906</v>
+        <v>912.0911904761907</v>
       </c>
     </row>
     <row r="480">
@@ -4349,7 +4349,7 @@
         <v>488</v>
       </c>
       <c r="B490" t="n">
-        <v>493.8283333333333</v>
+        <v>493.8283333333334</v>
       </c>
     </row>
     <row r="491">
@@ -4421,7 +4421,7 @@
         <v>497</v>
       </c>
       <c r="B499" t="n">
-        <v>336.8736666666666</v>
+        <v>336.8736666666667</v>
       </c>
     </row>
     <row r="500">
@@ -4445,7 +4445,7 @@
         <v>500</v>
       </c>
       <c r="B502" t="n">
-        <v>310.0716666666667</v>
+        <v>310.0716666666666</v>
       </c>
     </row>
     <row r="503">
@@ -4453,7 +4453,7 @@
         <v>501</v>
       </c>
       <c r="B503" t="n">
-        <v>280.4</v>
+        <v>280.4000000000001</v>
       </c>
     </row>
     <row r="504">
@@ -4501,7 +4501,7 @@
         <v>507</v>
       </c>
       <c r="B509" t="n">
-        <v>211.7944444444444</v>
+        <v>211.7944444444445</v>
       </c>
     </row>
     <row r="510">
@@ -4533,7 +4533,7 @@
         <v>511</v>
       </c>
       <c r="B513" t="n">
-        <v>2502.290666666666</v>
+        <v>2502.290666666667</v>
       </c>
     </row>
     <row r="514">
@@ -4565,7 +4565,7 @@
         <v>515</v>
       </c>
       <c r="B517" t="n">
-        <v>203.6016666666665</v>
+        <v>203.6016666666666</v>
       </c>
     </row>
     <row r="518">
@@ -4581,7 +4581,7 @@
         <v>517</v>
       </c>
       <c r="B519" t="n">
-        <v>608.8978333333333</v>
+        <v>608.8978333333334</v>
       </c>
     </row>
     <row r="520">
@@ -4821,7 +4821,7 @@
         <v>547</v>
       </c>
       <c r="B549" t="n">
-        <v>361.965</v>
+        <v>361.9649999999999</v>
       </c>
     </row>
     <row r="550">
@@ -4917,7 +4917,7 @@
         <v>559</v>
       </c>
       <c r="B561" t="n">
-        <v>604.1483492063493</v>
+        <v>604.1483492063492</v>
       </c>
     </row>
     <row r="562">
@@ -4981,7 +4981,7 @@
         <v>567</v>
       </c>
       <c r="B569" t="n">
-        <v>266.6513333333335</v>
+        <v>266.6513333333334</v>
       </c>
     </row>
     <row r="570">
@@ -5021,7 +5021,7 @@
         <v>572</v>
       </c>
       <c r="B574" t="n">
-        <v>298.0094523809526</v>
+        <v>298.0094523809525</v>
       </c>
     </row>
     <row r="575">
@@ -5165,7 +5165,7 @@
         <v>590</v>
       </c>
       <c r="B592" t="n">
-        <v>579.3869999999999</v>
+        <v>579.3870000000001</v>
       </c>
     </row>
     <row r="593">
@@ -5205,7 +5205,7 @@
         <v>595</v>
       </c>
       <c r="B597" t="n">
-        <v>466.5083333333334</v>
+        <v>466.5083333333333</v>
       </c>
     </row>
     <row r="598">
@@ -5213,7 +5213,7 @@
         <v>596</v>
       </c>
       <c r="B598" t="n">
-        <v>154.9333333333333</v>
+        <v>154.9333333333334</v>
       </c>
     </row>
     <row r="599">
@@ -5245,7 +5245,7 @@
         <v>600</v>
       </c>
       <c r="B602" t="n">
-        <v>330.8533888888891</v>
+        <v>330.853388888889</v>
       </c>
     </row>
     <row r="603">
@@ -5261,7 +5261,7 @@
         <v>602</v>
       </c>
       <c r="B604" t="n">
-        <v>808.05</v>
+        <v>808.0500000000001</v>
       </c>
     </row>
     <row r="605">
@@ -5293,7 +5293,7 @@
         <v>606</v>
       </c>
       <c r="B608" t="n">
-        <v>280.7928888888891</v>
+        <v>280.792888888889</v>
       </c>
     </row>
     <row r="609">
@@ -5309,7 +5309,7 @@
         <v>608</v>
       </c>
       <c r="B610" t="n">
-        <v>305.3105555555556</v>
+        <v>305.3105555555555</v>
       </c>
     </row>
     <row r="611">
@@ -5357,7 +5357,7 @@
         <v>614</v>
       </c>
       <c r="B616" t="n">
-        <v>414.9477777777779</v>
+        <v>414.9477777777778</v>
       </c>
     </row>
     <row r="617">
@@ -5389,7 +5389,7 @@
         <v>618</v>
       </c>
       <c r="B620" t="n">
-        <v>435.7589999999999</v>
+        <v>435.759</v>
       </c>
     </row>
     <row r="621">
@@ -5405,7 +5405,7 @@
         <v>620</v>
       </c>
       <c r="B622" t="n">
-        <v>298.82</v>
+        <v>298.8200000000001</v>
       </c>
     </row>
     <row r="623">
@@ -5445,7 +5445,7 @@
         <v>625</v>
       </c>
       <c r="B627" t="n">
-        <v>448.08825</v>
+        <v>448.0882500000001</v>
       </c>
     </row>
     <row r="628">
@@ -5557,7 +5557,7 @@
         <v>639</v>
       </c>
       <c r="B641" t="n">
-        <v>677.7906666666667</v>
+        <v>677.7906666666665</v>
       </c>
     </row>
     <row r="642">
@@ -5581,7 +5581,7 @@
         <v>642</v>
       </c>
       <c r="B644" t="n">
-        <v>559.0186666666666</v>
+        <v>559.0186666666667</v>
       </c>
     </row>
     <row r="645">
@@ -5605,7 +5605,7 @@
         <v>645</v>
       </c>
       <c r="B647" t="n">
-        <v>405.2166666666667</v>
+        <v>405.2166666666668</v>
       </c>
     </row>
     <row r="648">
@@ -5629,7 +5629,7 @@
         <v>648</v>
       </c>
       <c r="B650" t="n">
-        <v>608.8978333333333</v>
+        <v>608.8978333333334</v>
       </c>
     </row>
     <row r="651">
@@ -5717,7 +5717,7 @@
         <v>659</v>
       </c>
       <c r="B661" t="n">
-        <v>200.8016666666664</v>
+        <v>200.8016666666666</v>
       </c>
     </row>
     <row r="662">
@@ -5733,7 +5733,7 @@
         <v>661</v>
       </c>
       <c r="B663" t="n">
-        <v>267.7466666666665</v>
+        <v>267.7466666666666</v>
       </c>
     </row>
     <row r="664">
@@ -5741,7 +5741,7 @@
         <v>662</v>
       </c>
       <c r="B664" t="n">
-        <v>304.6169999999998</v>
+        <v>304.6169999999999</v>
       </c>
     </row>
     <row r="665">
@@ -5821,7 +5821,7 @@
         <v>672</v>
       </c>
       <c r="B674" t="n">
-        <v>404.7266666666667</v>
+        <v>404.7266666666666</v>
       </c>
     </row>
     <row r="675">
@@ -5965,7 +5965,7 @@
         <v>690</v>
       </c>
       <c r="B692" t="n">
-        <v>229.0283333333335</v>
+        <v>229.0283333333334</v>
       </c>
     </row>
     <row r="693">
@@ -5997,7 +5997,7 @@
         <v>694</v>
       </c>
       <c r="B696" t="n">
-        <v>455.5445555555556</v>
+        <v>455.5445555555555</v>
       </c>
     </row>
     <row r="697">
@@ -6109,7 +6109,7 @@
         <v>708</v>
       </c>
       <c r="B710" t="n">
-        <v>779.7018888888889</v>
+        <v>779.7018888888888</v>
       </c>
     </row>
     <row r="711">
@@ -6125,7 +6125,7 @@
         <v>710</v>
       </c>
       <c r="B712" t="n">
-        <v>433.9722916666666</v>
+        <v>433.9722916666667</v>
       </c>
     </row>
     <row r="713">
@@ -6165,7 +6165,7 @@
         <v>715</v>
       </c>
       <c r="B717" t="n">
-        <v>445.4286111111111</v>
+        <v>445.4286111111112</v>
       </c>
     </row>
     <row r="718">
@@ -6197,7 +6197,7 @@
         <v>719</v>
       </c>
       <c r="B721" t="n">
-        <v>720.2571904761905</v>
+        <v>720.2571904761904</v>
       </c>
     </row>
     <row r="722">
@@ -6349,7 +6349,7 @@
         <v>738</v>
       </c>
       <c r="B740" t="n">
-        <v>406.9466666666666</v>
+        <v>406.9466666666667</v>
       </c>
     </row>
     <row r="741">
@@ -6389,7 +6389,7 @@
         <v>743</v>
       </c>
       <c r="B745" t="n">
-        <v>287.6666666666665</v>
+        <v>287.6666666666666</v>
       </c>
     </row>
     <row r="746">
@@ -6429,7 +6429,7 @@
         <v>748</v>
       </c>
       <c r="B750" t="n">
-        <v>262.5848333333333</v>
+        <v>262.5848333333334</v>
       </c>
     </row>
     <row r="751">
@@ -6509,7 +6509,7 @@
         <v>758</v>
       </c>
       <c r="B760" t="n">
-        <v>261.3000000000001</v>
+        <v>261.3</v>
       </c>
     </row>
     <row r="761">
@@ -6541,7 +6541,7 @@
         <v>762</v>
       </c>
       <c r="B764" t="n">
-        <v>357.1166666666668</v>
+        <v>357.1166666666667</v>
       </c>
     </row>
     <row r="765">
@@ -6557,7 +6557,7 @@
         <v>764</v>
       </c>
       <c r="B766" t="n">
-        <v>834.1323333333333</v>
+        <v>834.1323333333335</v>
       </c>
     </row>
     <row r="767">
@@ -6581,7 +6581,7 @@
         <v>767</v>
       </c>
       <c r="B769" t="n">
-        <v>777.2736111111111</v>
+        <v>777.2736111111112</v>
       </c>
     </row>
     <row r="770">
@@ -6589,7 +6589,7 @@
         <v>768</v>
       </c>
       <c r="B770" t="n">
-        <v>789.5781999999999</v>
+        <v>789.5782</v>
       </c>
     </row>
     <row r="771">
@@ -6629,7 +6629,7 @@
         <v>773</v>
       </c>
       <c r="B775" t="n">
-        <v>375.7242539682539</v>
+        <v>375.7242539682541</v>
       </c>
     </row>
     <row r="776">
@@ -6637,7 +6637,7 @@
         <v>774</v>
       </c>
       <c r="B776" t="n">
-        <v>637.556</v>
+        <v>637.5559999999999</v>
       </c>
     </row>
     <row r="777">
@@ -6861,7 +6861,7 @@
         <v>802</v>
       </c>
       <c r="B804" t="n">
-        <v>493.6202222222223</v>
+        <v>493.6202222222222</v>
       </c>
     </row>
     <row r="805">
@@ -6941,7 +6941,7 @@
         <v>812</v>
       </c>
       <c r="B814" t="n">
-        <v>273.1166666666666</v>
+        <v>273.1166666666667</v>
       </c>
     </row>
     <row r="815">
@@ -6997,7 +6997,7 @@
         <v>819</v>
       </c>
       <c r="B821" t="n">
-        <v>288.4954999999999</v>
+        <v>288.4955</v>
       </c>
     </row>
     <row r="822">
@@ -7013,7 +7013,7 @@
         <v>821</v>
       </c>
       <c r="B823" t="n">
-        <v>448.08825</v>
+        <v>448.0882500000001</v>
       </c>
     </row>
     <row r="824">
@@ -7021,7 +7021,7 @@
         <v>822</v>
       </c>
       <c r="B824" t="n">
-        <v>456.3718333333334</v>
+        <v>456.3718333333333</v>
       </c>
     </row>
     <row r="825">
@@ -7061,7 +7061,7 @@
         <v>827</v>
       </c>
       <c r="B829" t="n">
-        <v>330.6453333333334</v>
+        <v>330.6453333333333</v>
       </c>
     </row>
     <row r="830">
@@ -7077,7 +7077,7 @@
         <v>829</v>
       </c>
       <c r="B831" t="n">
-        <v>344.0916666666666</v>
+        <v>344.0916666666667</v>
       </c>
     </row>
     <row r="832">
@@ -7197,7 +7197,7 @@
         <v>844</v>
       </c>
       <c r="B846" t="n">
-        <v>399.5616666666666</v>
+        <v>399.5616666666667</v>
       </c>
     </row>
     <row r="847">
@@ -7205,7 +7205,7 @@
         <v>845</v>
       </c>
       <c r="B847" t="n">
-        <v>724.9668333333333</v>
+        <v>724.9668333333332</v>
       </c>
     </row>
     <row r="848">
@@ -7373,7 +7373,7 @@
         <v>866</v>
       </c>
       <c r="B868" t="n">
-        <v>326.4591666666668</v>
+        <v>326.4591666666667</v>
       </c>
     </row>
     <row r="869">
@@ -7389,7 +7389,7 @@
         <v>868</v>
       </c>
       <c r="B870" t="n">
-        <v>705.5896666666667</v>
+        <v>705.5896666666666</v>
       </c>
     </row>
     <row r="871">
@@ -7405,7 +7405,7 @@
         <v>870</v>
       </c>
       <c r="B872" t="n">
-        <v>192.4686111111112</v>
+        <v>192.4686111111113</v>
       </c>
     </row>
     <row r="873">
@@ -7493,7 +7493,7 @@
         <v>881</v>
       </c>
       <c r="B883" t="n">
-        <v>399.0641666666667</v>
+        <v>399.0641666666666</v>
       </c>
     </row>
     <row r="884">
@@ -7533,7 +7533,7 @@
         <v>886</v>
       </c>
       <c r="B888" t="n">
-        <v>453.678</v>
+        <v>453.6779999999999</v>
       </c>
     </row>
     <row r="889">
@@ -7661,7 +7661,7 @@
         <v>902</v>
       </c>
       <c r="B904" t="n">
-        <v>488.5936666666666</v>
+        <v>488.5936666666667</v>
       </c>
     </row>
     <row r="905">
@@ -7717,7 +7717,7 @@
         <v>909</v>
       </c>
       <c r="B911" t="n">
-        <v>341.5119444444445</v>
+        <v>341.5119444444444</v>
       </c>
     </row>
     <row r="912">
@@ -7853,7 +7853,7 @@
         <v>926</v>
       </c>
       <c r="B928" t="n">
-        <v>310.5945</v>
+        <v>310.5945000000001</v>
       </c>
     </row>
     <row r="929">
@@ -7893,7 +7893,7 @@
         <v>931</v>
       </c>
       <c r="B933" t="n">
-        <v>912.0911904761906</v>
+        <v>912.0911904761907</v>
       </c>
     </row>
     <row r="934">
@@ -7917,7 +7917,7 @@
         <v>934</v>
       </c>
       <c r="B936" t="n">
-        <v>126.5000000000002</v>
+        <v>126.5000000000001</v>
       </c>
     </row>
     <row r="937">
@@ -7949,7 +7949,7 @@
         <v>938</v>
       </c>
       <c r="B940" t="n">
-        <v>307.0501666666668</v>
+        <v>307.0501666666667</v>
       </c>
     </row>
     <row r="941">
@@ -8061,7 +8061,7 @@
         <v>952</v>
       </c>
       <c r="B954" t="n">
-        <v>349.4799999999999</v>
+        <v>349.48</v>
       </c>
     </row>
     <row r="955">
@@ -8085,7 +8085,7 @@
         <v>955</v>
       </c>
       <c r="B957" t="n">
-        <v>195.4363333333336</v>
+        <v>195.4363333333337</v>
       </c>
     </row>
     <row r="958">
@@ -8133,7 +8133,7 @@
         <v>961</v>
       </c>
       <c r="B963" t="n">
-        <v>325.5766666666667</v>
+        <v>325.5766666666668</v>
       </c>
     </row>
     <row r="964">
@@ -8197,7 +8197,7 @@
         <v>969</v>
       </c>
       <c r="B971" t="n">
-        <v>493.8283333333333</v>
+        <v>493.8283333333334</v>
       </c>
     </row>
     <row r="972">
@@ -8205,7 +8205,7 @@
         <v>970</v>
       </c>
       <c r="B972" t="n">
-        <v>493.8283333333333</v>
+        <v>493.8283333333334</v>
       </c>
     </row>
     <row r="973">
@@ -8293,7 +8293,7 @@
         <v>981</v>
       </c>
       <c r="B983" t="n">
-        <v>855.1500000000001</v>
+        <v>855.15</v>
       </c>
     </row>
     <row r="984">
@@ -8381,7 +8381,7 @@
         <v>992</v>
       </c>
       <c r="B994" t="n">
-        <v>837.8189888888888</v>
+        <v>837.818988888889</v>
       </c>
     </row>
     <row r="995">
@@ -8397,7 +8397,7 @@
         <v>994</v>
       </c>
       <c r="B996" t="n">
-        <v>345.1093333333334</v>
+        <v>345.1093333333333</v>
       </c>
     </row>
     <row r="997">
@@ -8429,7 +8429,7 @@
         <v>998</v>
       </c>
       <c r="B1000" t="n">
-        <v>317.7341666666665</v>
+        <v>317.7341666666666</v>
       </c>
     </row>
     <row r="1001">
@@ -8613,7 +8613,7 @@
         <v>1021</v>
       </c>
       <c r="B1023" t="n">
-        <v>238.7859999999999</v>
+        <v>238.786</v>
       </c>
     </row>
     <row r="1024">
@@ -8629,7 +8629,7 @@
         <v>1023</v>
       </c>
       <c r="B1025" t="n">
-        <v>340.8179365079366</v>
+        <v>340.8179365079365</v>
       </c>
     </row>
     <row r="1026">
@@ -8637,7 +8637,7 @@
         <v>1024</v>
       </c>
       <c r="B1026" t="n">
-        <v>364.4366666666666</v>
+        <v>364.4366666666667</v>
       </c>
     </row>
     <row r="1027">
@@ -8869,7 +8869,7 @@
         <v>1053</v>
       </c>
       <c r="B1055" t="n">
-        <v>318.0863333333332</v>
+        <v>318.0863333333333</v>
       </c>
     </row>
     <row r="1056">
@@ -8965,7 +8965,7 @@
         <v>1065</v>
       </c>
       <c r="B1067" t="n">
-        <v>801.2873333333332</v>
+        <v>801.2873333333333</v>
       </c>
     </row>
     <row r="1068">
@@ -8989,7 +8989,7 @@
         <v>1068</v>
       </c>
       <c r="B1070" t="n">
-        <v>354.5613333333334</v>
+        <v>354.5613333333333</v>
       </c>
     </row>
     <row r="1071">
@@ -9077,7 +9077,7 @@
         <v>1079</v>
       </c>
       <c r="B1081" t="n">
-        <v>345.1650277777778</v>
+        <v>345.1650277777777</v>
       </c>
     </row>
     <row r="1082">
@@ -9109,7 +9109,7 @@
         <v>1083</v>
       </c>
       <c r="B1085" t="n">
-        <v>322.2499999999999</v>
+        <v>322.25</v>
       </c>
     </row>
     <row r="1086">
@@ -9141,7 +9141,7 @@
         <v>1087</v>
       </c>
       <c r="B1089" t="n">
-        <v>348.6979166666667</v>
+        <v>348.6979166666666</v>
       </c>
     </row>
     <row r="1090">
@@ -9165,7 +9165,7 @@
         <v>1090</v>
       </c>
       <c r="B1092" t="n">
-        <v>579.3869999999999</v>
+        <v>579.3870000000001</v>
       </c>
     </row>
     <row r="1093">
@@ -9197,7 +9197,7 @@
         <v>1094</v>
       </c>
       <c r="B1096" t="n">
-        <v>441.2916666666666</v>
+        <v>441.2916666666667</v>
       </c>
     </row>
     <row r="1097">
@@ -9285,7 +9285,7 @@
         <v>1105</v>
       </c>
       <c r="B1107" t="n">
-        <v>305.1007222222223</v>
+        <v>305.1007222222222</v>
       </c>
     </row>
     <row r="1108">
@@ -9349,7 +9349,7 @@
         <v>1113</v>
       </c>
       <c r="B1115" t="n">
-        <v>417.15</v>
+        <v>417.1500000000001</v>
       </c>
     </row>
     <row r="1116">
@@ -9405,7 +9405,7 @@
         <v>1120</v>
       </c>
       <c r="B1122" t="n">
-        <v>311.7260555555556</v>
+        <v>311.7260555555555</v>
       </c>
     </row>
     <row r="1123">
@@ -9413,7 +9413,7 @@
         <v>1121</v>
       </c>
       <c r="B1123" t="n">
-        <v>668.9516666666667</v>
+        <v>668.9516666666666</v>
       </c>
     </row>
     <row r="1124">
@@ -9573,7 +9573,7 @@
         <v>1141</v>
       </c>
       <c r="B1143" t="n">
-        <v>827.6162777777777</v>
+        <v>827.6162777777778</v>
       </c>
     </row>
     <row r="1144">
@@ -9669,7 +9669,7 @@
         <v>1153</v>
       </c>
       <c r="B1155" t="n">
-        <v>286.8266666666667</v>
+        <v>286.8266666666666</v>
       </c>
     </row>
     <row r="1156">
@@ -9685,7 +9685,7 @@
         <v>1155</v>
       </c>
       <c r="B1157" t="n">
-        <v>879.6043333333332</v>
+        <v>879.6043333333333</v>
       </c>
     </row>
     <row r="1158">
@@ -9693,7 +9693,7 @@
         <v>1156</v>
       </c>
       <c r="B1158" t="n">
-        <v>371.5166666666668</v>
+        <v>371.5166666666667</v>
       </c>
     </row>
     <row r="1159">
@@ -9909,7 +9909,7 @@
         <v>1183</v>
       </c>
       <c r="B1185" t="n">
-        <v>279.4540000000002</v>
+        <v>279.4540000000001</v>
       </c>
     </row>
     <row r="1186">
@@ -9989,7 +9989,7 @@
         <v>1193</v>
       </c>
       <c r="B1195" t="n">
-        <v>319.4133333333333</v>
+        <v>319.4133333333334</v>
       </c>
     </row>
     <row r="1196">
@@ -10013,7 +10013,7 @@
         <v>1196</v>
       </c>
       <c r="B1198" t="n">
-        <v>711.0976666666668</v>
+        <v>711.0976666666667</v>
       </c>
     </row>
     <row r="1199">
@@ -10061,7 +10061,7 @@
         <v>1202</v>
       </c>
       <c r="B1204" t="n">
-        <v>132.6000000000001</v>
+        <v>132.6</v>
       </c>
     </row>
     <row r="1205">
@@ -10205,7 +10205,7 @@
         <v>1220</v>
       </c>
       <c r="B1222" t="n">
-        <v>282.425</v>
+        <v>282.4249999999998</v>
       </c>
     </row>
     <row r="1223">
@@ -10221,7 +10221,7 @@
         <v>1222</v>
       </c>
       <c r="B1224" t="n">
-        <v>146.7999999999999</v>
+        <v>146.8</v>
       </c>
     </row>
     <row r="1225">
@@ -10269,7 +10269,7 @@
         <v>1228</v>
       </c>
       <c r="B1230" t="n">
-        <v>329.9805555555556</v>
+        <v>329.9805555555557</v>
       </c>
     </row>
     <row r="1231">
@@ -10349,7 +10349,7 @@
         <v>1238</v>
       </c>
       <c r="B1240" t="n">
-        <v>329.7753333333333</v>
+        <v>329.7753333333334</v>
       </c>
     </row>
     <row r="1241">
@@ -10405,7 +10405,7 @@
         <v>1245</v>
       </c>
       <c r="B1247" t="n">
-        <v>296.0333333333333</v>
+        <v>296.0333333333332</v>
       </c>
     </row>
     <row r="1248">
@@ -10421,7 +10421,7 @@
         <v>1247</v>
       </c>
       <c r="B1249" t="n">
-        <v>290.5261111111111</v>
+        <v>290.5261111111112</v>
       </c>
     </row>
     <row r="1250">
@@ -10485,7 +10485,7 @@
         <v>1255</v>
       </c>
       <c r="B1257" t="n">
-        <v>493.8283333333333</v>
+        <v>493.8283333333334</v>
       </c>
     </row>
     <row r="1258">
@@ -10493,7 +10493,7 @@
         <v>1256</v>
       </c>
       <c r="B1258" t="n">
-        <v>327.3058333333335</v>
+        <v>327.3058333333334</v>
       </c>
     </row>
     <row r="1259">
@@ -10501,7 +10501,7 @@
         <v>1257</v>
       </c>
       <c r="B1259" t="n">
-        <v>790.2</v>
+        <v>790.1999999999999</v>
       </c>
     </row>
     <row r="1260">
@@ -10509,7 +10509,7 @@
         <v>1258</v>
       </c>
       <c r="B1260" t="n">
-        <v>283.6677777777778</v>
+        <v>283.6677777777777</v>
       </c>
     </row>
     <row r="1261">
@@ -10525,7 +10525,7 @@
         <v>1260</v>
       </c>
       <c r="B1262" t="n">
-        <v>349.4356666666666</v>
+        <v>349.4356666666665</v>
       </c>
     </row>
     <row r="1263">
@@ -10541,7 +10541,7 @@
         <v>1262</v>
       </c>
       <c r="B1264" t="n">
-        <v>474.6813648148147</v>
+        <v>474.6813648148148</v>
       </c>
     </row>
     <row r="1265">
@@ -10565,7 +10565,7 @@
         <v>1265</v>
       </c>
       <c r="B1267" t="n">
-        <v>329.3993333333333</v>
+        <v>329.3993333333332</v>
       </c>
     </row>
     <row r="1268">
@@ -10589,7 +10589,7 @@
         <v>1268</v>
       </c>
       <c r="B1270" t="n">
-        <v>952.1913333333333</v>
+        <v>952.1913333333332</v>
       </c>
     </row>
     <row r="1271">
@@ -10597,7 +10597,7 @@
         <v>1269</v>
       </c>
       <c r="B1271" t="n">
-        <v>781.5553888888887</v>
+        <v>781.5553888888888</v>
       </c>
     </row>
     <row r="1272">
@@ -10605,7 +10605,7 @@
         <v>1270</v>
       </c>
       <c r="B1272" t="n">
-        <v>541.3938611111111</v>
+        <v>541.3938611111112</v>
       </c>
     </row>
     <row r="1273">
@@ -10613,7 +10613,7 @@
         <v>1271</v>
       </c>
       <c r="B1273" t="n">
-        <v>285.7833333333334</v>
+        <v>285.7833333333335</v>
       </c>
     </row>
     <row r="1274">
@@ -10629,7 +10629,7 @@
         <v>1273</v>
       </c>
       <c r="B1275" t="n">
-        <v>401.5333333333333</v>
+        <v>401.5333333333334</v>
       </c>
     </row>
     <row r="1276">
@@ -10645,7 +10645,7 @@
         <v>1275</v>
       </c>
       <c r="B1277" t="n">
-        <v>396.2069999999999</v>
+        <v>396.207</v>
       </c>
     </row>
     <row r="1278">
@@ -10741,7 +10741,7 @@
         <v>1287</v>
       </c>
       <c r="B1289" t="n">
-        <v>1254.242833333333</v>
+        <v>1254.242833333334</v>
       </c>
     </row>
     <row r="1290">
@@ -10749,7 +10749,7 @@
         <v>1288</v>
       </c>
       <c r="B1290" t="n">
-        <v>407.8100000000001</v>
+        <v>407.8099999999999</v>
       </c>
     </row>
     <row r="1291">
@@ -10909,7 +10909,7 @@
         <v>1308</v>
       </c>
       <c r="B1310" t="n">
-        <v>714.1621666666666</v>
+        <v>714.1621666666665</v>
       </c>
     </row>
     <row r="1311">
@@ -10965,7 +10965,7 @@
         <v>1315</v>
       </c>
       <c r="B1317" t="n">
-        <v>407.5272222222221</v>
+        <v>407.5272222222222</v>
       </c>
     </row>
     <row r="1318">
@@ -11045,7 +11045,7 @@
         <v>1325</v>
       </c>
       <c r="B1327" t="n">
-        <v>385.7215</v>
+        <v>385.7215000000001</v>
       </c>
     </row>
     <row r="1328">
@@ -11165,7 +11165,7 @@
         <v>1340</v>
       </c>
       <c r="B1342" t="n">
-        <v>164.6208333333332</v>
+        <v>164.6208333333333</v>
       </c>
     </row>
     <row r="1343">
@@ -11181,7 +11181,7 @@
         <v>1342</v>
       </c>
       <c r="B1344" t="n">
-        <v>691.9566666666667</v>
+        <v>691.9566666666666</v>
       </c>
     </row>
     <row r="1345">
@@ -11205,7 +11205,7 @@
         <v>1345</v>
       </c>
       <c r="B1347" t="n">
-        <v>391.5696111111111</v>
+        <v>391.5696111111112</v>
       </c>
     </row>
     <row r="1348">
@@ -11333,7 +11333,7 @@
         <v>1361</v>
       </c>
       <c r="B1363" t="n">
-        <v>448.08825</v>
+        <v>448.0882500000001</v>
       </c>
     </row>
     <row r="1364">
@@ -11373,7 +11373,7 @@
         <v>1366</v>
       </c>
       <c r="B1368" t="n">
-        <v>798</v>
+        <v>797.9999999999999</v>
       </c>
     </row>
     <row r="1369">
@@ -11461,7 +11461,7 @@
         <v>1377</v>
       </c>
       <c r="B1379" t="n">
-        <v>331.2624999999999</v>
+        <v>331.2625</v>
       </c>
     </row>
     <row r="1380">
@@ -11477,7 +11477,7 @@
         <v>1379</v>
       </c>
       <c r="B1381" t="n">
-        <v>417.5011111111111</v>
+        <v>417.5011111111112</v>
       </c>
     </row>
     <row r="1382">
@@ -11493,7 +11493,7 @@
         <v>1381</v>
       </c>
       <c r="B1383" t="n">
-        <v>341.7833333333334</v>
+        <v>341.7833333333333</v>
       </c>
     </row>
     <row r="1384">
@@ -11509,7 +11509,7 @@
         <v>1383</v>
       </c>
       <c r="B1385" t="n">
-        <v>722.9313083333333</v>
+        <v>722.9313083333334</v>
       </c>
     </row>
     <row r="1386">
@@ -11605,7 +11605,7 @@
         <v>1395</v>
       </c>
       <c r="B1397" t="n">
-        <v>310.2950000000001</v>
+        <v>310.295</v>
       </c>
     </row>
     <row r="1398">
@@ -11629,7 +11629,7 @@
         <v>1398</v>
       </c>
       <c r="B1400" t="n">
-        <v>263.1226666666669</v>
+        <v>263.1226666666668</v>
       </c>
     </row>
     <row r="1401">
@@ -11669,7 +11669,7 @@
         <v>1403</v>
       </c>
       <c r="B1405" t="n">
-        <v>205.3</v>
+        <v>205.2999999999999</v>
       </c>
     </row>
     <row r="1406">
@@ -11701,7 +11701,7 @@
         <v>1407</v>
       </c>
       <c r="B1409" t="n">
-        <v>330.6453333333334</v>
+        <v>330.6453333333333</v>
       </c>
     </row>
     <row r="1410">
@@ -11829,7 +11829,7 @@
         <v>1423</v>
       </c>
       <c r="B1425" t="n">
-        <v>505.2116666666666</v>
+        <v>505.2116666666667</v>
       </c>
     </row>
     <row r="1426">
@@ -11869,7 +11869,7 @@
         <v>1428</v>
       </c>
       <c r="B1430" t="n">
-        <v>950.2582916666664</v>
+        <v>950.2582916666665</v>
       </c>
     </row>
     <row r="1431">
@@ -11893,7 +11893,7 @@
         <v>1431</v>
       </c>
       <c r="B1433" t="n">
-        <v>267.2425555555557</v>
+        <v>267.2425555555556</v>
       </c>
     </row>
     <row r="1434">
@@ -11941,7 +11941,7 @@
         <v>1437</v>
       </c>
       <c r="B1439" t="n">
-        <v>247.8411111111114</v>
+        <v>247.8411111111113</v>
       </c>
     </row>
     <row r="1440">
@@ -11965,7 +11965,7 @@
         <v>1440</v>
       </c>
       <c r="B1442" t="n">
-        <v>498.6696666666666</v>
+        <v>498.6696666666667</v>
       </c>
     </row>
     <row r="1443">
@@ -12029,7 +12029,7 @@
         <v>1448</v>
       </c>
       <c r="B1450" t="n">
-        <v>225.8469761904761</v>
+        <v>225.846976190476</v>
       </c>
     </row>
     <row r="1451">
@@ -12133,7 +12133,7 @@
         <v>1461</v>
       </c>
       <c r="B1463" t="n">
-        <v>1149.039666666667</v>
+        <v>1149.039666666666</v>
       </c>
     </row>
     <row r="1464">
@@ -12189,7 +12189,7 @@
         <v>1468</v>
       </c>
       <c r="B1470" t="n">
-        <v>473.0204999999999</v>
+        <v>473.0205</v>
       </c>
     </row>
     <row r="1471">
@@ -12205,7 +12205,7 @@
         <v>1470</v>
       </c>
       <c r="B1472" t="n">
-        <v>400.7765555555557</v>
+        <v>400.7765555555556</v>
       </c>
     </row>
     <row r="1473">
@@ -12237,7 +12237,7 @@
         <v>1474</v>
       </c>
       <c r="B1476" t="n">
-        <v>363.6619999999999</v>
+        <v>363.662</v>
       </c>
     </row>
     <row r="1477">
@@ -12245,7 +12245,7 @@
         <v>1475</v>
       </c>
       <c r="B1477" t="n">
-        <v>302.6926190476191</v>
+        <v>302.692619047619</v>
       </c>
     </row>
     <row r="1478">
@@ -12269,7 +12269,7 @@
         <v>1478</v>
       </c>
       <c r="B1480" t="n">
-        <v>449.1395</v>
+        <v>449.1394999999999</v>
       </c>
     </row>
     <row r="1481">
@@ -12285,7 +12285,7 @@
         <v>1480</v>
       </c>
       <c r="B1482" t="n">
-        <v>831.8629999999999</v>
+        <v>831.8629999999998</v>
       </c>
     </row>
     <row r="1483">
@@ -12397,7 +12397,7 @@
         <v>1494</v>
       </c>
       <c r="B1496" t="n">
-        <v>406.6486111111111</v>
+        <v>406.648611111111</v>
       </c>
     </row>
     <row r="1497">
@@ -12421,7 +12421,7 @@
         <v>1497</v>
       </c>
       <c r="B1499" t="n">
-        <v>1243.136166666667</v>
+        <v>1243.136166666666</v>
       </c>
     </row>
     <row r="1500">
@@ -12469,7 +12469,7 @@
         <v>1503</v>
       </c>
       <c r="B1505" t="n">
-        <v>341.2833333333334</v>
+        <v>341.2833333333333</v>
       </c>
     </row>
     <row r="1506">
@@ -12477,7 +12477,7 @@
         <v>1504</v>
       </c>
       <c r="B1506" t="n">
-        <v>319.904</v>
+        <v>319.9039999999999</v>
       </c>
     </row>
     <row r="1507">
@@ -12573,7 +12573,7 @@
         <v>1516</v>
       </c>
       <c r="B1518" t="n">
-        <v>283.3553333333333</v>
+        <v>283.3553333333332</v>
       </c>
     </row>
     <row r="1519">
@@ -12781,7 +12781,7 @@
         <v>1542</v>
       </c>
       <c r="B1544" t="n">
-        <v>310.8728333333332</v>
+        <v>310.8728333333333</v>
       </c>
     </row>
     <row r="1545">
@@ -12829,7 +12829,7 @@
         <v>1548</v>
       </c>
       <c r="B1550" t="n">
-        <v>375.7242539682539</v>
+        <v>375.7242539682541</v>
       </c>
     </row>
     <row r="1551">
@@ -12885,7 +12885,7 @@
         <v>1555</v>
       </c>
       <c r="B1557" t="n">
-        <v>620.5397222222222</v>
+        <v>620.5397222222223</v>
       </c>
     </row>
     <row r="1558">

</xml_diff>